<commit_message>
Cleaned up the Parts List
</commit_message>
<xml_diff>
--- a/OrbitalShaker_PartsList.xlsx
+++ b/OrbitalShaker_PartsList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Electronics Parts" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="292">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -449,7 +449,7 @@
     <t xml:space="preserve">KJ-201BD</t>
   </si>
   <si>
-    <t xml:space="preserve">M4 nut</t>
+    <t xml:space="preserve">M4 Nut</t>
   </si>
   <si>
     <t xml:space="preserve">M4 zinc-plated steel nut (pack of 100)</t>
@@ -464,7 +464,7 @@
     <t xml:space="preserve">M4-HFST-Z100-</t>
   </si>
   <si>
-    <t xml:space="preserve">M4 washer</t>
+    <t xml:space="preserve">M4 Washer</t>
   </si>
   <si>
     <t xml:space="preserve">M4 zinc-plated steel washer (pack of 100)</t>
@@ -476,7 +476,7 @@
     <t xml:space="preserve">DM4-FASTWAZ100DIN125</t>
   </si>
   <si>
-    <t xml:space="preserve">M4×12 screw</t>
+    <t xml:space="preserve">M4×12 Screw</t>
   </si>
   <si>
     <t xml:space="preserve">M4 12mm zinc-plated pan head screw (pack of 100)</t>
@@ -488,7 +488,7 @@
     <t xml:space="preserve">M4 12 PRSTMC Z100</t>
   </si>
   <si>
-    <t xml:space="preserve">M3×10 screw</t>
+    <t xml:space="preserve">M3×10 Screw</t>
   </si>
   <si>
     <t xml:space="preserve">M3 10mm countersunk zinc-plated screw (pack of 100)</t>
@@ -525,6 +525,18 @@
   </si>
   <si>
     <t xml:space="preserve">2214009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40mm Fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 VDC Fan, 60mA, 40mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2816685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC002106</t>
   </si>
   <si>
     <t xml:space="preserve">30V/1A AC Adaptor</t>
@@ -737,6 +749,129 @@
     <t xml:space="preserve">All Purpose</t>
   </si>
   <si>
+    <t xml:space="preserve">Scissors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common scissors (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B00XP1V0UU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxford 13cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fine tip permanent marker pen (not black, any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staedtler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B005DPPQAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruler 30 cm (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q Connect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B000NMBTUK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldering Equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tweezers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watchmakers tweezers (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duratool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3127692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1PK-125T-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solder Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solder flux (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chip Quik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1850220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD291NL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solder Wire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thin solder wire (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3262209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D03341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldering Station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldering station suitable for SMD (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metcal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1560738</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS-900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isopropyl alcohol for cleaning (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexeal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B079YVPZDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small Tub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margarine tub or something similar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old toothbrush or stiff paintbrush</t>
+  </si>
+  <si>
     <t xml:space="preserve">Electrical Tape</t>
   </si>
   <si>
@@ -747,136 +882,6 @@
   </si>
   <si>
     <t xml:space="preserve">PVC TAPE 1920B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scissors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Common scissors (any make)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Helix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B00XP1V0UU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxford 13cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fine tip permanent marker pen (not black, any make)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Staedtler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B005DPPQAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ruler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ruler 30 cm (any make)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q Connect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B000NMBTUK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soldering Equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tweezers</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Watchmakers tweezers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (any make)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Duratool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3127692</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1PK-125T-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solder Flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solder flux (any make)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chip Quik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1850220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD291NL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solder Wire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thin solder wire (any make)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3262209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D03341</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soldering Station</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soldering station suitable for SMD (any make)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metcal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1560738</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PS-900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isopropyl alcohol for cleaning (any make)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hexeal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B079YVPZDF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3D Printing</t>
   </si>
   <si>
     <t xml:space="preserve">3D Printer</t>
@@ -959,7 +964,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1001,11 +1006,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1107,7 +1107,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1147,7 +1147,7 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2242,16 +2242,16 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.1"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.89"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
@@ -2342,7 +2342,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2579,20 +2579,20 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2668,7 +2668,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>167</v>
@@ -2680,20 +2680,20 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="I3" s="1" t="n">
-        <v>23.37</v>
+        <v>2.11</v>
       </c>
       <c r="J3" s="1" t="n">
         <f aca="false">I3*B3</f>
-        <v>23.37</v>
+        <v>8.44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2702,32 +2702,32 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0.73</v>
+        <v>23.37</v>
       </c>
       <c r="J4" s="1" t="n">
         <f aca="false">I4*B4</f>
-        <v>2.92</v>
+        <v>23.37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2739,22 +2739,22 @@
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="I5" s="11" t="n">
         <v>35.71</v>
@@ -2773,22 +2773,22 @@
         <v>2</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="I6" s="11" t="n">
         <v>0.315</v>
@@ -2807,22 +2807,22 @@
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>179</v>
-      </c>
       <c r="G7" s="12" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="I7" s="11" t="n">
         <v>0.315</v>
@@ -2841,22 +2841,22 @@
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="I8" s="11" t="n">
         <v>32.72</v>
@@ -2875,22 +2875,22 @@
         <v>1</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="I9" s="11" t="n">
         <v>2.01</v>
@@ -2914,14 +2914,14 @@
       <c r="I10" s="1"/>
       <c r="J10" s="5" t="n">
         <f aca="false">SUM(J2:J9)</f>
-        <v>149.67</v>
+        <v>155.19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="2214009"/>
-    <hyperlink ref="G3" r:id="rId2" display="2771453"/>
-    <hyperlink ref="G4" r:id="rId3" display="1466738"/>
+    <hyperlink ref="G3" r:id="rId2" display="2816685"/>
+    <hyperlink ref="G4" r:id="rId3" display="2771453"/>
     <hyperlink ref="G5" r:id="rId4" display="4621906"/>
     <hyperlink ref="G6" r:id="rId5" display="2528081"/>
     <hyperlink ref="G7" r:id="rId6" display="2528174"/>
@@ -2943,10 +2943,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2955,11 +2955,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="52.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2997,7 +2997,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -3018,22 +3018,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I3" s="16" t="n">
         <v>8.77</v>
@@ -3052,22 +3052,22 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="I4" s="16" t="n">
         <v>10.71</v>
@@ -3086,22 +3086,22 @@
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="I5" s="17" t="n">
         <v>108.59</v>
@@ -3120,22 +3120,22 @@
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I6" s="17" t="n">
         <v>30</v>
@@ -3147,7 +3147,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -3168,22 +3168,22 @@
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="I8" s="17" t="n">
         <v>1.58</v>
@@ -3202,29 +3202,29 @@
         <v>1</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>12</v>
-      </c>
       <c r="F9" s="9" t="s">
-        <v>179</v>
+        <v>225</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="I9" s="17" t="n">
-        <v>1.18</v>
+        <v>1.39</v>
       </c>
       <c r="J9" s="17" t="n">
         <f aca="false">I9*B9</f>
-        <v>1.18</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3236,29 +3236,29 @@
         <v>1</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>227</v>
+        <v>231</v>
+      </c>
+      <c r="H10" s="11" t="n">
+        <v>733449</v>
       </c>
       <c r="I10" s="17" t="n">
-        <v>1.39</v>
+        <v>1.66</v>
       </c>
       <c r="J10" s="17" t="n">
         <f aca="false">I10*B10</f>
-        <v>1.39</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3270,111 +3270,111 @@
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="H11" s="11" t="n">
-        <v>733449</v>
+        <v>235</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>232</v>
       </c>
       <c r="I11" s="17" t="n">
-        <v>1.66</v>
+        <v>0.59</v>
       </c>
       <c r="J11" s="17" t="n">
         <f aca="false">I11*B11</f>
-        <v>1.66</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="n">
+      <c r="A12" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="n">
         <f aca="false">1+A11</f>
         <v>9</v>
       </c>
-      <c r="B12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="I12" s="17" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="J12" s="17" t="n">
-        <f aca="false">I12*B12</f>
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="B13" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="I13" s="17" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="J13" s="17" t="n">
+        <f aca="false">I13*B13</f>
+        <v>3.22</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="n">
-        <f aca="false">1+A12</f>
+        <f aca="false">1+A13</f>
         <v>10</v>
       </c>
       <c r="B14" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="I14" s="17" t="n">
-        <v>3.22</v>
+        <v>11.94</v>
       </c>
       <c r="J14" s="17" t="n">
         <f aca="false">I14*B14</f>
-        <v>3.22</v>
+        <v>11.94</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3386,29 +3386,29 @@
         <v>1</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="I15" s="17" t="n">
-        <v>11.94</v>
+        <v>5.18</v>
       </c>
       <c r="J15" s="17" t="n">
         <f aca="false">I15*B15</f>
-        <v>11.94</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3420,70 +3420,48 @@
         <v>1</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="I16" s="17" t="n">
-        <v>5.18</v>
+        <v>187</v>
       </c>
       <c r="J16" s="17" t="n">
         <f aca="false">I16*B16</f>
-        <v>5.18</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="n">
+      <c r="A17" s="15"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="n">
         <f aca="false">1+A16</f>
         <v>13</v>
       </c>
-      <c r="B17" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="I17" s="17" t="n">
-        <v>187</v>
-      </c>
-      <c r="J17" s="17" t="n">
-        <f aca="false">I17*B17</f>
-        <v>187</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="n">
-        <f aca="false">1+A17</f>
-        <v>14</v>
-      </c>
       <c r="B18" s="18" t="n">
         <v>1</v>
       </c>
@@ -3494,7 +3472,7 @@
         <v>257</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>258</v>
@@ -3514,59 +3492,80 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="n">
+        <f aca="false">1+A18</f>
+        <v>14</v>
+      </c>
+      <c r="B19" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
+      <c r="D19" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="n">
-        <f aca="false">1+A18</f>
+        <f aca="false">1+A19</f>
         <v>15</v>
       </c>
       <c r="B20" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E20" s="9"/>
-      <c r="F20" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>264</v>
-      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="9"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="15" t="n">
+        <f aca="false">1+A20</f>
+        <v>16</v>
+      </c>
+      <c r="B21" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="E21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="I21" s="17" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="J21" s="17" t="n">
+        <f aca="false">I21*B21</f>
+        <v>1.18</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="n">
@@ -3577,178 +3576,218 @@
         <v>1</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>215</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="E22" s="9"/>
       <c r="F22" s="9" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="I22" s="17" t="n">
-        <v>44.99</v>
-      </c>
-      <c r="J22" s="17" t="n">
-        <f aca="false">I22*B22</f>
-        <v>44.99</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="n">
+      <c r="A23" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15" t="n">
         <f aca="false">1+A22</f>
         <v>17</v>
       </c>
-      <c r="B23" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="G23" s="12" t="s">
+      <c r="B24" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="I23" s="17" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="J23" s="17" t="n">
-        <f aca="false">I23*B23</f>
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15" t="n">
-        <f aca="false">1+A23</f>
-        <v>18</v>
-      </c>
-      <c r="B24" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="E24" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="G24" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="G24" s="12" t="s">
+      <c r="H24" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="H24" s="9" t="s">
-        <v>278</v>
-      </c>
       <c r="I24" s="17" t="n">
-        <v>7.32</v>
+        <v>44.99</v>
       </c>
       <c r="J24" s="17" t="n">
         <f aca="false">I24*B24</f>
-        <v>7.32</v>
+        <v>44.99</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="n">
         <f aca="false">1+A24</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="E25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G25" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="F25" s="9" t="s">
+      <c r="H25" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="G25" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="H25" s="11" t="n">
-        <v>20150</v>
-      </c>
       <c r="I25" s="17" t="n">
-        <v>4.49</v>
+        <v>0.44</v>
       </c>
       <c r="J25" s="17" t="n">
         <f aca="false">I25*B25</f>
-        <v>4.49</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="15" t="n">
         <f aca="false">1+A25</f>
+        <v>19</v>
+      </c>
+      <c r="B26" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="I26" s="17" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="J26" s="17" t="n">
+        <f aca="false">I26*B26</f>
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="15" t="n">
+        <f aca="false">1+A26</f>
         <v>20</v>
       </c>
-      <c r="B26" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="H27" s="11" t="n">
+        <v>20150</v>
+      </c>
+      <c r="I27" s="17" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="J27" s="17" t="n">
+        <f aca="false">I27*B27</f>
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="15" t="n">
+        <f aca="false">1+A27</f>
+        <v>21</v>
+      </c>
+      <c r="B28" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="5" t="n">
-        <f aca="false">SUM(J3:J26)</f>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="5" t="n">
+        <f aca="false">SUM(J3:J28)</f>
         <v>435.84</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A7:J7"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A19:J19"/>
-    <mergeCell ref="A21:J21"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A23:J23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" display="375238"/>
@@ -3756,20 +3795,20 @@
     <hyperlink ref="G5" r:id="rId3" display="829-6561"/>
     <hyperlink ref="G6" r:id="rId4" display="123-1930"/>
     <hyperlink ref="G8" r:id="rId5" display="B0001OZI48"/>
-    <hyperlink ref="G9" r:id="rId6" display="152346"/>
-    <hyperlink ref="G10" r:id="rId7" display="B00XP1V0UU"/>
-    <hyperlink ref="G11" r:id="rId8" display="B005DPPQAG"/>
-    <hyperlink ref="G12" r:id="rId9" display="B000NMBTUK"/>
-    <hyperlink ref="G14" r:id="rId10" display="3127692"/>
-    <hyperlink ref="G15" r:id="rId11" display="1850220"/>
-    <hyperlink ref="G16" r:id="rId12" display="3262209"/>
-    <hyperlink ref="G17" r:id="rId13" display="1560738"/>
-    <hyperlink ref="G18" r:id="rId14" display="B079YVPZDF"/>
-    <hyperlink ref="G20" r:id="rId15" display="uPrint SE Plus"/>
-    <hyperlink ref="G22" r:id="rId16" display="B00IINANZ8"/>
-    <hyperlink ref="G23" r:id="rId17" display="378124"/>
-    <hyperlink ref="G24" r:id="rId18" display="2103261"/>
-    <hyperlink ref="G25" r:id="rId19" display="B001PNBC0I"/>
+    <hyperlink ref="G9" r:id="rId6" display="B00XP1V0UU"/>
+    <hyperlink ref="G10" r:id="rId7" display="B005DPPQAG"/>
+    <hyperlink ref="G11" r:id="rId8" display="B000NMBTUK"/>
+    <hyperlink ref="G13" r:id="rId9" display="3127692"/>
+    <hyperlink ref="G14" r:id="rId10" display="1850220"/>
+    <hyperlink ref="G15" r:id="rId11" display="3262209"/>
+    <hyperlink ref="G16" r:id="rId12" display="1560738"/>
+    <hyperlink ref="G18" r:id="rId13" display="B079YVPZDF"/>
+    <hyperlink ref="G21" r:id="rId14" display="152346"/>
+    <hyperlink ref="G22" r:id="rId15" display="uPrint SE Plus"/>
+    <hyperlink ref="G24" r:id="rId16" display="B00IINANZ8"/>
+    <hyperlink ref="G25" r:id="rId17" display="378124"/>
+    <hyperlink ref="G26" r:id="rId18" display="2103261"/>
+    <hyperlink ref="G27" r:id="rId19" display="B001PNBC0I"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>